<commit_message>
Universal Code edit 2
</commit_message>
<xml_diff>
--- a/Facility Staffing Combined.xlsx
+++ b/Facility Staffing Combined.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keros\.venv\Capstone-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDABD2BD-8129-43A5-A1AA-1171D29DFE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A96448-3831-400B-9295-4AAE1BC46704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0B339019-6CC6-4650-AC0A-9ED3E400C083}"/>
+    <workbookView xWindow="-17670" yWindow="1260" windowWidth="16410" windowHeight="11295" xr2:uid="{0B339019-6CC6-4650-AC0A-9ED3E400C083}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,192 +36,195 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+  <si>
+    <t>Q1 2021</t>
+  </si>
+  <si>
+    <t>Q2 2021</t>
+  </si>
+  <si>
+    <t>Q3 2021</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q4 2021 </t>
+  </si>
+  <si>
+    <t>Q1 2022</t>
+  </si>
+  <si>
+    <t>Q2 2022</t>
+  </si>
+  <si>
+    <t>Q3 2022</t>
+  </si>
+  <si>
+    <t>Q4 2022</t>
+  </si>
+  <si>
+    <t>Q1 2023</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Staff Average </t>
+  </si>
+  <si>
+    <t>Staff Increase/Decrease</t>
+  </si>
+  <si>
+    <t>Alabama</t>
+  </si>
+  <si>
+    <t>Alaska</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
+    <t>Arkansas</t>
+  </si>
+  <si>
+    <t>California</t>
+  </si>
+  <si>
+    <t>Colorado</t>
+  </si>
+  <si>
+    <t>Connecticut</t>
+  </si>
+  <si>
+    <t>Delaware</t>
+  </si>
+  <si>
+    <t>District of Columbia</t>
+  </si>
+  <si>
+    <t>Florida</t>
+  </si>
+  <si>
+    <t>Georgia</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>Idaho</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>Indiana</t>
+  </si>
+  <si>
+    <t>Iowa</t>
+  </si>
+  <si>
+    <t>Kansas</t>
+  </si>
+  <si>
+    <t>Kentucky</t>
+  </si>
+  <si>
+    <t>Louisiana</t>
+  </si>
+  <si>
+    <t>Maine</t>
+  </si>
+  <si>
+    <t>Maryland</t>
+  </si>
+  <si>
+    <t>Massachusetts</t>
+  </si>
+  <si>
+    <t>Michigan</t>
+  </si>
+  <si>
+    <t>Minnesota</t>
+  </si>
+  <si>
+    <t>Mississippi</t>
+  </si>
+  <si>
+    <t>Missouri</t>
+  </si>
+  <si>
+    <t>Montana</t>
+  </si>
+  <si>
+    <t>Nebraska</t>
+  </si>
+  <si>
+    <t>Nevada</t>
+  </si>
+  <si>
+    <t>New Hampshire</t>
+  </si>
+  <si>
+    <t>New Jersey</t>
+  </si>
+  <si>
+    <t>New Mexico</t>
+  </si>
+  <si>
+    <t>New York</t>
+  </si>
+  <si>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>North Dakota</t>
+  </si>
+  <si>
+    <t>Ohio</t>
+  </si>
+  <si>
+    <t>Oklahoma</t>
+  </si>
+  <si>
+    <t>Oregon</t>
+  </si>
+  <si>
+    <t>Pennsylvania</t>
+  </si>
+  <si>
+    <t>Rhode Island</t>
+  </si>
+  <si>
+    <t>South Carolina</t>
+  </si>
+  <si>
+    <t>South Dakota</t>
+  </si>
+  <si>
+    <t>Tennessee</t>
+  </si>
+  <si>
+    <t>Texas</t>
+  </si>
+  <si>
+    <t>Utah</t>
+  </si>
+  <si>
+    <t>Vermont</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>Washington</t>
+  </si>
+  <si>
+    <t>West Virginia</t>
+  </si>
+  <si>
+    <t>Wisconsin</t>
+  </si>
+  <si>
+    <t>Wyoming</t>
+  </si>
   <si>
     <t>State</t>
-  </si>
-  <si>
-    <t>ALASKA</t>
-  </si>
-  <si>
-    <t>ALABAMA</t>
-  </si>
-  <si>
-    <t>ARKANSAS</t>
-  </si>
-  <si>
-    <t>ARIZONA</t>
-  </si>
-  <si>
-    <t>CALIFORNIA</t>
-  </si>
-  <si>
-    <t>COLORADO</t>
-  </si>
-  <si>
-    <t>CONNECTICUT</t>
-  </si>
-  <si>
-    <t>D.C.</t>
-  </si>
-  <si>
-    <t>DELAWARE</t>
-  </si>
-  <si>
-    <t>FLORIDA</t>
-  </si>
-  <si>
-    <t>GEORGIA</t>
-  </si>
-  <si>
-    <t>HAWAII</t>
-  </si>
-  <si>
-    <t>IOWA</t>
-  </si>
-  <si>
-    <t>IDAHO</t>
-  </si>
-  <si>
-    <t>ILLINOIS</t>
-  </si>
-  <si>
-    <t>INDIANA</t>
-  </si>
-  <si>
-    <t>KANSAS</t>
-  </si>
-  <si>
-    <t>KENTUCKY</t>
-  </si>
-  <si>
-    <t>LOUISIANA</t>
-  </si>
-  <si>
-    <t>MASSACHUSETTS</t>
-  </si>
-  <si>
-    <t>MARYLAND</t>
-  </si>
-  <si>
-    <t>MAINE</t>
-  </si>
-  <si>
-    <t>MICHIGAN</t>
-  </si>
-  <si>
-    <t>MINNESOTA</t>
-  </si>
-  <si>
-    <t>MISSOURI</t>
-  </si>
-  <si>
-    <t>MISSISSIPPI</t>
-  </si>
-  <si>
-    <t>MONTANA</t>
-  </si>
-  <si>
-    <t>NORTH CAROLINA</t>
-  </si>
-  <si>
-    <t>NORTH DAKOTA</t>
-  </si>
-  <si>
-    <t>NEBRASKA</t>
-  </si>
-  <si>
-    <t>NEW HAMPSHIRE</t>
-  </si>
-  <si>
-    <t>NEW JERSEY</t>
-  </si>
-  <si>
-    <t>NEW MEXICO</t>
-  </si>
-  <si>
-    <t>NEVADA</t>
-  </si>
-  <si>
-    <t>NEW YORK</t>
-  </si>
-  <si>
-    <t>OHIO</t>
-  </si>
-  <si>
-    <t>OKLAHOMA</t>
-  </si>
-  <si>
-    <t>OREGON</t>
-  </si>
-  <si>
-    <t>PENNSYLVANIA</t>
-  </si>
-  <si>
-    <t>RHODE ISLAND</t>
-  </si>
-  <si>
-    <t>SOUTH CAROLINA</t>
-  </si>
-  <si>
-    <t>SOUTH DAKOTA</t>
-  </si>
-  <si>
-    <t>TENNESSEE</t>
-  </si>
-  <si>
-    <t>TEXAS</t>
-  </si>
-  <si>
-    <t>UTAH</t>
-  </si>
-  <si>
-    <t>VIRGINIA</t>
-  </si>
-  <si>
-    <t>VERMONT</t>
-  </si>
-  <si>
-    <t>WASHINGTON</t>
-  </si>
-  <si>
-    <t>WISCONSIN</t>
-  </si>
-  <si>
-    <t>WEST VIRGINIA</t>
-  </si>
-  <si>
-    <t>WYOMING</t>
-  </si>
-  <si>
-    <t>Q1 2021</t>
-  </si>
-  <si>
-    <t>Q2 2021</t>
-  </si>
-  <si>
-    <t>Q3 2021</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Q4 2021 </t>
-  </si>
-  <si>
-    <t>Q1 2022</t>
-  </si>
-  <si>
-    <t>Q2 2022</t>
-  </si>
-  <si>
-    <t>Q3 2022</t>
-  </si>
-  <si>
-    <t>Q4 2022</t>
-  </si>
-  <si>
-    <t>Q1 2023</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Average </t>
   </si>
 </sst>
 </file>
@@ -265,11 +268,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B72183B1-1C58-4195-9159-864865B1E67C}">
-  <dimension ref="A1:K53"/>
+  <dimension ref="A1:L53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="O39" sqref="O39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,47 +599,51 @@
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>52</v>
-      </c>
       <c r="C1" t="s">
-        <v>53</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>54</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>55</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>56</v>
+        <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>57</v>
+        <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>58</v>
+        <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>60</v>
+        <v>8</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>468</v>
@@ -668,10 +676,14 @@
         <f>(B2+C2+D2+E2+F2+G2+H2+I2+J2)/9</f>
         <v>581.77777777777783</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="4">
+        <f>(J2-B2)/J2</f>
+        <v>0.25119999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B3" s="1">
         <v>18523</v>
@@ -704,10 +716,14 @@
         <f t="shared" ref="K3:K42" si="0">(B3+C3+D3+E3+F3+G3+H3+I3+J3)/9</f>
         <v>19238.777777777777</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" s="4">
+        <f t="shared" ref="L3:L52" si="1">(J3-B3)/J3</f>
+        <v>9.6174490094661849E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="B4" s="1">
         <v>13620</v>
@@ -740,10 +756,14 @@
         <f t="shared" si="0"/>
         <v>14836.111111111111</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" s="4">
+        <f t="shared" si="1"/>
+        <v>0.13093415007656967</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1">
         <v>10231</v>
@@ -776,10 +796,14 @@
         <f t="shared" si="0"/>
         <v>10633.444444444445</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" s="4">
+        <f t="shared" si="1"/>
+        <v>0.10419402854391034</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B6" s="1">
         <v>83713</v>
@@ -812,10 +836,14 @@
         <f t="shared" si="0"/>
         <v>91049.222222222219</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="4">
+        <f t="shared" si="1"/>
+        <v>0.1425659619796788</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B7" s="1">
         <v>13227</v>
@@ -848,10 +876,14 @@
         <f t="shared" si="0"/>
         <v>14047.555555555555</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="4">
+        <f t="shared" si="1"/>
+        <v>8.5396210759231095E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B8" s="1">
         <v>17823</v>
@@ -884,10 +916,14 @@
         <f t="shared" si="0"/>
         <v>18894.222222222223</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="4">
+        <f t="shared" si="1"/>
+        <v>0.10148215366001211</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1">
         <v>1910</v>
@@ -920,10 +956,14 @@
         <f t="shared" si="0"/>
         <v>1976.2222222222222</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="4">
+        <f t="shared" si="1"/>
+        <v>3.7783375314861464E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B10" s="1">
         <v>3276</v>
@@ -956,10 +996,14 @@
         <f t="shared" si="0"/>
         <v>3475.5555555555557</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="4">
+        <f t="shared" si="1"/>
+        <v>0.10393873085339168</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="B11" s="1">
         <v>63887</v>
@@ -992,10 +1036,14 @@
         <f t="shared" si="0"/>
         <v>66926.888888888891</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="4">
+        <f t="shared" si="1"/>
+        <v>0.11008497005153921</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B12" s="1">
         <v>26814</v>
@@ -1028,10 +1076,14 @@
         <f t="shared" si="0"/>
         <v>27631</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" s="4">
+        <f t="shared" si="1"/>
+        <v>8.7928160821796664E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B13" s="1">
         <v>3181</v>
@@ -1064,10 +1116,14 @@
         <f t="shared" si="0"/>
         <v>3159.6666666666665</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" s="4">
+        <f t="shared" si="1"/>
+        <v>-1.5644955300127713E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B14" s="1">
         <v>19036</v>
@@ -1100,10 +1156,14 @@
         <f t="shared" si="0"/>
         <v>19686</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" s="4">
+        <f t="shared" si="1"/>
+        <v>3.8731505327475636E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B15" s="1">
         <v>3585</v>
@@ -1136,10 +1196,14 @@
         <f t="shared" si="0"/>
         <v>3657.8888888888887</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" s="4">
+        <f t="shared" si="1"/>
+        <v>9.1024340770791079E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B16" s="1">
         <v>52141</v>
@@ -1172,10 +1236,14 @@
         <f t="shared" si="0"/>
         <v>56573.555555555555</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="4">
+        <f t="shared" si="1"/>
+        <v>0.12966332270610426</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B17" s="1">
         <v>31955</v>
@@ -1208,10 +1276,14 @@
         <f t="shared" si="0"/>
         <v>33906.777777777781</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" s="4">
+        <f t="shared" si="1"/>
+        <v>8.9886360399874687E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B18" s="1">
         <v>13903</v>
@@ -1244,10 +1316,14 @@
         <f t="shared" si="0"/>
         <v>14469.888888888889</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="4">
+        <f t="shared" si="1"/>
+        <v>5.2671027527936766E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="B19" s="1">
         <v>19024</v>
@@ -1280,10 +1356,14 @@
         <f t="shared" si="0"/>
         <v>20069.666666666668</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" s="4">
+        <f t="shared" si="1"/>
+        <v>6.845558711193811E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="B20" s="1">
         <v>20902</v>
@@ -1316,10 +1396,14 @@
         <f t="shared" si="0"/>
         <v>21796.555555555555</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" s="4">
+        <f t="shared" si="1"/>
+        <v>7.3287519397029488E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="B21" s="1">
         <v>29866</v>
@@ -1352,10 +1436,14 @@
         <f t="shared" si="0"/>
         <v>31527.888888888891</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" s="4">
+        <f t="shared" si="1"/>
+        <v>8.3471429448229301E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="B22" s="1">
         <v>19785</v>
@@ -1388,10 +1476,14 @@
         <f t="shared" si="0"/>
         <v>21272.888888888891</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" s="4">
+        <f t="shared" si="1"/>
+        <v>0.12011918527083519</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="B23" s="1">
         <v>4865</v>
@@ -1424,10 +1516,14 @@
         <f t="shared" si="0"/>
         <v>4887.1111111111113</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" s="4">
+        <f t="shared" si="1"/>
+        <v>4.4579732914375489E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="B24" s="1">
         <v>30334</v>
@@ -1460,10 +1556,14 @@
         <f t="shared" si="0"/>
         <v>31645.777777777777</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" s="4">
+        <f t="shared" si="1"/>
+        <v>9.0979922085705725E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B25" s="1">
         <v>19600</v>
@@ -1496,10 +1596,14 @@
         <f t="shared" si="0"/>
         <v>19658.444444444445</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" s="4">
+        <f t="shared" si="1"/>
+        <v>1.7149734229264867E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B26" s="1">
         <v>29130</v>
@@ -1532,10 +1636,14 @@
         <f t="shared" si="0"/>
         <v>31743.222222222223</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" s="4">
+        <f t="shared" si="1"/>
+        <v>0.12961634994621729</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B27" s="1">
         <v>13027</v>
@@ -1568,10 +1676,14 @@
         <f t="shared" si="0"/>
         <v>13617</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L27" s="4">
+        <f t="shared" si="1"/>
+        <v>7.864771200226324E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B28" s="1">
         <v>3151</v>
@@ -1604,10 +1716,14 @@
         <f t="shared" si="0"/>
         <v>3158.6666666666665</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L28" s="4">
+        <f t="shared" si="1"/>
+        <v>6.6204287515762928E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="B29" s="1">
         <v>28564</v>
@@ -1640,10 +1756,14 @@
         <f t="shared" si="0"/>
         <v>31356</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L29" s="4">
+        <f t="shared" si="1"/>
+        <v>0.12999512670565302</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B30" s="1">
         <v>4236</v>
@@ -1676,10 +1796,14 @@
         <f t="shared" si="0"/>
         <v>4445.666666666667</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L30" s="4">
+        <f t="shared" si="1"/>
+        <v>4.9584922593672871E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="B31" s="1">
         <v>9098</v>
@@ -1712,10 +1836,14 @@
         <f t="shared" si="0"/>
         <v>9359.2222222222226</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L31" s="4">
+        <f t="shared" si="1"/>
+        <v>3.2642211589580007E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="B32" s="1">
         <v>5322</v>
@@ -1748,10 +1876,14 @@
         <f t="shared" si="0"/>
         <v>5484.7777777777774</v>
       </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L32" s="4">
+        <f t="shared" si="1"/>
+        <v>6.004945249028612E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="B33" s="1">
         <v>35152</v>
@@ -1784,10 +1916,14 @@
         <f t="shared" si="0"/>
         <v>37192.111111111109</v>
       </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L33" s="4">
+        <f t="shared" si="1"/>
+        <v>0.10842823445861972</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="B34" s="1">
         <v>4502</v>
@@ -1820,10 +1956,14 @@
         <f t="shared" si="0"/>
         <v>4855.333333333333</v>
       </c>
-    </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L34" s="4">
+        <f t="shared" si="1"/>
+        <v>0.1169085916045508</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B35" s="1">
         <v>4774</v>
@@ -1856,10 +1996,14 @@
         <f t="shared" si="0"/>
         <v>5124.5555555555557</v>
       </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L35" s="4">
+        <f t="shared" si="1"/>
+        <v>0.13373253493013973</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B36" s="1">
         <v>86862</v>
@@ -1892,10 +2036,14 @@
         <f t="shared" si="0"/>
         <v>92205.555555555562</v>
       </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L36" s="4">
+        <f t="shared" si="1"/>
+        <v>9.6711798839458407E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="B37" s="1">
         <v>58717</v>
@@ -1928,10 +2076,14 @@
         <f t="shared" si="0"/>
         <v>62399.111111111109</v>
       </c>
-    </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L37" s="4">
+        <f t="shared" si="1"/>
+        <v>9.668933263591889E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="B38" s="1">
         <v>14369</v>
@@ -1964,10 +2116,14 @@
         <f t="shared" si="0"/>
         <v>15212.222222222223</v>
       </c>
-    </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L38" s="4">
+        <f t="shared" si="1"/>
+        <v>9.0742264127064487E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="B39" s="1">
         <v>6374</v>
@@ -2000,10 +2156,14 @@
         <f t="shared" si="0"/>
         <v>6165.1111111111113</v>
       </c>
-    </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L39" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.8562207519767631E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="B40" s="1">
         <v>61032</v>
@@ -2036,10 +2196,14 @@
         <f t="shared" si="0"/>
         <v>63692.777777777781</v>
       </c>
-    </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L40" s="4">
+        <f t="shared" si="1"/>
+        <v>7.2617039704608657E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B41" s="1">
         <v>5958</v>
@@ -2072,10 +2236,14 @@
         <f t="shared" si="0"/>
         <v>6467.333333333333</v>
       </c>
-    </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L41" s="4">
+        <f t="shared" si="1"/>
+        <v>0.13413748001743933</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B42" s="1">
         <v>14289</v>
@@ -2108,10 +2276,14 @@
         <f t="shared" si="0"/>
         <v>15117.111111111111</v>
       </c>
-    </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L42" s="4">
+        <f t="shared" si="1"/>
+        <v>9.7973612776971156E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B43" s="1">
         <v>4516</v>
@@ -2141,13 +2313,17 @@
         <v>4782</v>
       </c>
       <c r="K43" s="3">
-        <f>(B43+C43+D43+E43+F43+G43+H43+I42+J42)/9</f>
+        <f t="shared" ref="K43:K52" si="2">(B43+C43+D43+E43+F43+G43+H43+I42+J42)/9</f>
         <v>7072.333333333333</v>
       </c>
-    </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L43" s="4">
+        <f t="shared" si="1"/>
+        <v>5.562526139690506E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B44" s="1">
         <v>22355</v>
@@ -2177,13 +2353,17 @@
         <v>24327</v>
       </c>
       <c r="K44" s="3">
-        <f>(B44+C44+D44+E44+F44+G44+H44+I43+J43)/9</f>
+        <f t="shared" si="2"/>
         <v>19224.555555555555</v>
       </c>
-    </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L44" s="4">
+        <f t="shared" si="1"/>
+        <v>8.1062194269741442E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="B45" s="1">
         <v>75001</v>
@@ -2213,13 +2393,17 @@
         <v>84056</v>
       </c>
       <c r="K45" s="3">
-        <f>(B45+C45+D45+E45+F45+G45+H45+I44+J44)/9</f>
+        <f t="shared" si="2"/>
         <v>66427.888888888891</v>
       </c>
-    </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L45" s="4">
+        <f t="shared" si="1"/>
+        <v>0.10772580184638812</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B46" s="1">
         <v>4922</v>
@@ -2249,13 +2433,17 @@
         <v>5581</v>
       </c>
       <c r="K46" s="3">
-        <f>(B46+C46+D46+E46+F46+G46+H46+I45+J45)/9</f>
+        <f t="shared" si="2"/>
         <v>22662.666666666668</v>
       </c>
-    </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L46" s="4">
+        <f t="shared" si="1"/>
+        <v>0.11807919727647374</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="B47" s="1">
         <v>23540</v>
@@ -2285,13 +2473,17 @@
         <v>27078</v>
       </c>
       <c r="K47" s="3">
-        <f>(B47+C47+D47+E47+F47+G47+H47+I46+J46)/9</f>
+        <f t="shared" si="2"/>
         <v>20842.444444444445</v>
       </c>
-    </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L47" s="4">
+        <f t="shared" si="1"/>
+        <v>0.13065957603958933</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="B48" s="1">
         <v>2113</v>
@@ -2321,13 +2513,17 @@
         <v>2307</v>
       </c>
       <c r="K48" s="3">
-        <f>(B48+C48+D48+E48+F48+G48+H48+I47+J47)/9</f>
+        <f t="shared" si="2"/>
         <v>7728.1111111111113</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L48" s="4">
+        <f t="shared" si="1"/>
+        <v>8.4091894234937153E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B49" s="1">
         <v>11733</v>
@@ -2357,13 +2553,17 @@
         <v>12924</v>
       </c>
       <c r="K49" s="3">
-        <f>(B49+C49+D49+E49+F49+G49+H49+I48+J48)/9</f>
+        <f t="shared" si="2"/>
         <v>9989.4444444444453</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L49" s="4">
+        <f t="shared" si="1"/>
+        <v>9.2154131847725168E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
       <c r="B50" s="1">
         <v>17804</v>
@@ -2393,13 +2593,17 @@
         <v>17229</v>
       </c>
       <c r="K50" s="3">
-        <f>(B50+C50+D50+E50+F50+G50+H50+I49+J49)/9</f>
+        <f t="shared" si="2"/>
         <v>16504.555555555555</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L50" s="4">
+        <f t="shared" si="1"/>
+        <v>-3.3373962505078646E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="B51" s="1">
         <v>8249</v>
@@ -2429,13 +2633,17 @@
         <v>9226</v>
       </c>
       <c r="K51" s="3">
-        <f>(B51+C51+D51+E51+F51+G51+H51+I50+J50)/9</f>
+        <f t="shared" si="2"/>
         <v>10618.111111111111</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L51" s="4">
+        <f t="shared" si="1"/>
+        <v>0.10589637979622805</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B52" s="1">
         <v>1922</v>
@@ -2465,11 +2673,15 @@
         <v>1989</v>
       </c>
       <c r="K52" s="3">
-        <f>(B52+C52+D52+E52+F52+G52+H52+I51+J51)/9</f>
+        <f t="shared" si="2"/>
         <v>3555.5555555555557</v>
       </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L52" s="4">
+        <f t="shared" si="1"/>
+        <v>3.3685268979386625E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K53" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Facility staffing combined edited
</commit_message>
<xml_diff>
--- a/Facility Staffing Combined.xlsx
+++ b/Facility Staffing Combined.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keros\.venv\Capstone-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A96448-3831-400B-9295-4AAE1BC46704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CF0DAA-59BD-4C9E-BDD7-B5ED153FDBCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17670" yWindow="1260" windowWidth="16410" windowHeight="11295" xr2:uid="{0B339019-6CC6-4650-AC0A-9ED3E400C083}"/>
+    <workbookView xWindow="28545" yWindow="15480" windowWidth="16410" windowHeight="11295" xr2:uid="{0B339019-6CC6-4650-AC0A-9ED3E400C083}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,9 +65,6 @@
     <t>Q1 2023</t>
   </si>
   <si>
-    <t xml:space="preserve">Staff Average </t>
-  </si>
-  <si>
     <t>Staff Increase/Decrease</t>
   </si>
   <si>
@@ -225,22 +222,17 @@
   </si>
   <si>
     <t>State</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Employee Average </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -271,9 +263,9 @@
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,10 +580,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B72183B1-1C58-4195-9159-864865B1E67C}">
-  <dimension ref="A1:L53"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -599,13 +591,13 @@
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -634,16 +626,16 @@
       <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L1" t="s">
         <v>9</v>
-      </c>
-      <c r="L1" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2">
         <v>468</v>
@@ -672,18 +664,18 @@
       <c r="J2">
         <v>625</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="4">
         <f>(B2+C2+D2+E2+F2+G2+H2+I2+J2)/9</f>
         <v>581.77777777777783</v>
       </c>
-      <c r="L2" s="4">
+      <c r="L2" s="2">
         <f>(J2-B2)/J2</f>
         <v>0.25119999999999998</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1">
         <v>18523</v>
@@ -712,18 +704,18 @@
       <c r="J3" s="1">
         <v>20494</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K3" s="4">
         <f t="shared" ref="K3:K42" si="0">(B3+C3+D3+E3+F3+G3+H3+I3+J3)/9</f>
         <v>19238.777777777777</v>
       </c>
-      <c r="L3" s="4">
+      <c r="L3" s="2">
         <f t="shared" ref="L3:L52" si="1">(J3-B3)/J3</f>
         <v>9.6174490094661849E-2</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="1">
         <v>13620</v>
@@ -752,18 +744,18 @@
       <c r="J4" s="1">
         <v>15672</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4" s="4">
         <f t="shared" si="0"/>
         <v>14836.111111111111</v>
       </c>
-      <c r="L4" s="4">
+      <c r="L4" s="2">
         <f t="shared" si="1"/>
         <v>0.13093415007656967</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" s="1">
         <v>10231</v>
@@ -792,18 +784,18 @@
       <c r="J5" s="1">
         <v>11421</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5" s="4">
         <f t="shared" si="0"/>
         <v>10633.444444444445</v>
       </c>
-      <c r="L5" s="4">
+      <c r="L5" s="2">
         <f t="shared" si="1"/>
         <v>0.10419402854391034</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B6" s="1">
         <v>83713</v>
@@ -832,18 +824,18 @@
       <c r="J6" s="1">
         <v>97632</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="4">
         <f t="shared" si="0"/>
         <v>91049.222222222219</v>
       </c>
-      <c r="L6" s="4">
+      <c r="L6" s="2">
         <f t="shared" si="1"/>
         <v>0.1425659619796788</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1">
         <v>13227</v>
@@ -872,18 +864,18 @@
       <c r="J7" s="1">
         <v>14462</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7" s="4">
         <f t="shared" si="0"/>
         <v>14047.555555555555</v>
       </c>
-      <c r="L7" s="4">
+      <c r="L7" s="2">
         <f t="shared" si="1"/>
         <v>8.5396210759231095E-2</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="1">
         <v>17823</v>
@@ -912,18 +904,18 @@
       <c r="J8" s="1">
         <v>19836</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="4">
         <f t="shared" si="0"/>
         <v>18894.222222222223</v>
       </c>
-      <c r="L8" s="4">
+      <c r="L8" s="2">
         <f t="shared" si="1"/>
         <v>0.10148215366001211</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="1">
         <v>1910</v>
@@ -952,18 +944,18 @@
       <c r="J9" s="1">
         <v>1985</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="4">
         <f t="shared" si="0"/>
         <v>1976.2222222222222</v>
       </c>
-      <c r="L9" s="4">
+      <c r="L9" s="2">
         <f t="shared" si="1"/>
         <v>3.7783375314861464E-2</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1">
         <v>3276</v>
@@ -992,18 +984,18 @@
       <c r="J10" s="1">
         <v>3656</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10" s="4">
         <f t="shared" si="0"/>
         <v>3475.5555555555557</v>
       </c>
-      <c r="L10" s="4">
+      <c r="L10" s="2">
         <f t="shared" si="1"/>
         <v>0.10393873085339168</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1">
         <v>63887</v>
@@ -1032,18 +1024,18 @@
       <c r="J11" s="1">
         <v>71790</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11" s="4">
         <f t="shared" si="0"/>
         <v>66926.888888888891</v>
       </c>
-      <c r="L11" s="4">
+      <c r="L11" s="2">
         <f t="shared" si="1"/>
         <v>0.11008497005153921</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1">
         <v>26814</v>
@@ -1072,18 +1064,18 @@
       <c r="J12" s="1">
         <v>29399</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12" s="4">
         <f t="shared" si="0"/>
         <v>27631</v>
       </c>
-      <c r="L12" s="4">
+      <c r="L12" s="2">
         <f t="shared" si="1"/>
         <v>8.7928160821796664E-2</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" s="1">
         <v>3181</v>
@@ -1112,18 +1104,18 @@
       <c r="J13" s="1">
         <v>3132</v>
       </c>
-      <c r="K13" s="3">
+      <c r="K13" s="4">
         <f t="shared" si="0"/>
         <v>3159.6666666666665</v>
       </c>
-      <c r="L13" s="4">
+      <c r="L13" s="2">
         <f t="shared" si="1"/>
         <v>-1.5644955300127713E-2</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1">
         <v>19036</v>
@@ -1152,18 +1144,18 @@
       <c r="J14" s="1">
         <v>19803</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14" s="4">
         <f t="shared" si="0"/>
         <v>19686</v>
       </c>
-      <c r="L14" s="4">
+      <c r="L14" s="2">
         <f t="shared" si="1"/>
         <v>3.8731505327475636E-2</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B15" s="1">
         <v>3585</v>
@@ -1192,18 +1184,18 @@
       <c r="J15" s="1">
         <v>3944</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K15" s="4">
         <f t="shared" si="0"/>
         <v>3657.8888888888887</v>
       </c>
-      <c r="L15" s="4">
+      <c r="L15" s="2">
         <f t="shared" si="1"/>
         <v>9.1024340770791079E-2</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" s="1">
         <v>52141</v>
@@ -1232,18 +1224,18 @@
       <c r="J16" s="1">
         <v>59909</v>
       </c>
-      <c r="K16" s="3">
+      <c r="K16" s="4">
         <f t="shared" si="0"/>
         <v>56573.555555555555</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L16" s="2">
         <f t="shared" si="1"/>
         <v>0.12966332270610426</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B17" s="1">
         <v>31955</v>
@@ -1272,18 +1264,18 @@
       <c r="J17" s="1">
         <v>35111</v>
       </c>
-      <c r="K17" s="3">
+      <c r="K17" s="4">
         <f t="shared" si="0"/>
         <v>33906.777777777781</v>
       </c>
-      <c r="L17" s="4">
+      <c r="L17" s="2">
         <f t="shared" si="1"/>
         <v>8.9886360399874687E-2</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B18" s="1">
         <v>13903</v>
@@ -1312,18 +1304,18 @@
       <c r="J18" s="1">
         <v>14676</v>
       </c>
-      <c r="K18" s="3">
+      <c r="K18" s="4">
         <f t="shared" si="0"/>
         <v>14469.888888888889</v>
       </c>
-      <c r="L18" s="4">
+      <c r="L18" s="2">
         <f t="shared" si="1"/>
         <v>5.2671027527936766E-2</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B19" s="1">
         <v>19024</v>
@@ -1352,18 +1344,18 @@
       <c r="J19" s="1">
         <v>20422</v>
       </c>
-      <c r="K19" s="3">
+      <c r="K19" s="4">
         <f t="shared" si="0"/>
         <v>20069.666666666668</v>
       </c>
-      <c r="L19" s="4">
+      <c r="L19" s="2">
         <f t="shared" si="1"/>
         <v>6.845558711193811E-2</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B20" s="1">
         <v>20902</v>
@@ -1392,18 +1384,18 @@
       <c r="J20" s="1">
         <v>22555</v>
       </c>
-      <c r="K20" s="3">
+      <c r="K20" s="4">
         <f t="shared" si="0"/>
         <v>21796.555555555555</v>
       </c>
-      <c r="L20" s="4">
+      <c r="L20" s="2">
         <f t="shared" si="1"/>
         <v>7.3287519397029488E-2</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B21" s="1">
         <v>29866</v>
@@ -1432,18 +1424,18 @@
       <c r="J21" s="1">
         <v>32586</v>
       </c>
-      <c r="K21" s="3">
+      <c r="K21" s="4">
         <f t="shared" si="0"/>
         <v>31527.888888888891</v>
       </c>
-      <c r="L21" s="4">
+      <c r="L21" s="2">
         <f t="shared" si="1"/>
         <v>8.3471429448229301E-2</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B22" s="1">
         <v>19785</v>
@@ -1472,18 +1464,18 @@
       <c r="J22" s="1">
         <v>22486</v>
       </c>
-      <c r="K22" s="3">
+      <c r="K22" s="4">
         <f t="shared" si="0"/>
         <v>21272.888888888891</v>
       </c>
-      <c r="L22" s="4">
+      <c r="L22" s="2">
         <f t="shared" si="1"/>
         <v>0.12011918527083519</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B23" s="1">
         <v>4865</v>
@@ -1512,18 +1504,18 @@
       <c r="J23" s="1">
         <v>5092</v>
       </c>
-      <c r="K23" s="3">
+      <c r="K23" s="4">
         <f t="shared" si="0"/>
         <v>4887.1111111111113</v>
       </c>
-      <c r="L23" s="4">
+      <c r="L23" s="2">
         <f t="shared" si="1"/>
         <v>4.4579732914375489E-2</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" s="1">
         <v>30334</v>
@@ -1552,18 +1544,18 @@
       <c r="J24" s="1">
         <v>33370</v>
       </c>
-      <c r="K24" s="3">
+      <c r="K24" s="4">
         <f t="shared" si="0"/>
         <v>31645.777777777777</v>
       </c>
-      <c r="L24" s="4">
+      <c r="L24" s="2">
         <f t="shared" si="1"/>
         <v>9.0979922085705725E-2</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="1">
         <v>19600</v>
@@ -1592,18 +1584,18 @@
       <c r="J25" s="1">
         <v>19942</v>
       </c>
-      <c r="K25" s="3">
+      <c r="K25" s="4">
         <f t="shared" si="0"/>
         <v>19658.444444444445</v>
       </c>
-      <c r="L25" s="4">
+      <c r="L25" s="2">
         <f t="shared" si="1"/>
         <v>1.7149734229264867E-2</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B26" s="1">
         <v>29130</v>
@@ -1632,18 +1624,18 @@
       <c r="J26" s="1">
         <v>33468</v>
       </c>
-      <c r="K26" s="3">
+      <c r="K26" s="4">
         <f t="shared" si="0"/>
         <v>31743.222222222223</v>
       </c>
-      <c r="L26" s="4">
+      <c r="L26" s="2">
         <f t="shared" si="1"/>
         <v>0.12961634994621729</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B27" s="1">
         <v>13027</v>
@@ -1672,18 +1664,18 @@
       <c r="J27" s="1">
         <v>14139</v>
       </c>
-      <c r="K27" s="3">
+      <c r="K27" s="4">
         <f t="shared" si="0"/>
         <v>13617</v>
       </c>
-      <c r="L27" s="4">
+      <c r="L27" s="2">
         <f t="shared" si="1"/>
         <v>7.864771200226324E-2</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B28" s="1">
         <v>3151</v>
@@ -1712,18 +1704,18 @@
       <c r="J28" s="1">
         <v>3172</v>
       </c>
-      <c r="K28" s="3">
+      <c r="K28" s="4">
         <f t="shared" si="0"/>
         <v>3158.6666666666665</v>
       </c>
-      <c r="L28" s="4">
+      <c r="L28" s="2">
         <f t="shared" si="1"/>
         <v>6.6204287515762928E-3</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B29" s="1">
         <v>28564</v>
@@ -1752,18 +1744,18 @@
       <c r="J29" s="1">
         <v>32832</v>
       </c>
-      <c r="K29" s="3">
+      <c r="K29" s="4">
         <f t="shared" si="0"/>
         <v>31356</v>
       </c>
-      <c r="L29" s="4">
+      <c r="L29" s="2">
         <f t="shared" si="1"/>
         <v>0.12999512670565302</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B30" s="1">
         <v>4236</v>
@@ -1792,18 +1784,18 @@
       <c r="J30" s="1">
         <v>4457</v>
       </c>
-      <c r="K30" s="3">
+      <c r="K30" s="4">
         <f t="shared" si="0"/>
         <v>4445.666666666667</v>
       </c>
-      <c r="L30" s="4">
+      <c r="L30" s="2">
         <f t="shared" si="1"/>
         <v>4.9584922593672871E-2</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B31" s="1">
         <v>9098</v>
@@ -1832,18 +1824,18 @@
       <c r="J31" s="1">
         <v>9405</v>
       </c>
-      <c r="K31" s="3">
+      <c r="K31" s="4">
         <f t="shared" si="0"/>
         <v>9359.2222222222226</v>
       </c>
-      <c r="L31" s="4">
+      <c r="L31" s="2">
         <f t="shared" si="1"/>
         <v>3.2642211589580007E-2</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" s="1">
         <v>5322</v>
@@ -1872,18 +1864,18 @@
       <c r="J32" s="1">
         <v>5662</v>
       </c>
-      <c r="K32" s="3">
+      <c r="K32" s="4">
         <f t="shared" si="0"/>
         <v>5484.7777777777774</v>
       </c>
-      <c r="L32" s="4">
+      <c r="L32" s="2">
         <f t="shared" si="1"/>
         <v>6.004945249028612E-2</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B33" s="1">
         <v>35152</v>
@@ -1912,18 +1904,18 @@
       <c r="J33" s="1">
         <v>39427</v>
       </c>
-      <c r="K33" s="3">
+      <c r="K33" s="4">
         <f t="shared" si="0"/>
         <v>37192.111111111109</v>
       </c>
-      <c r="L33" s="4">
+      <c r="L33" s="2">
         <f t="shared" si="1"/>
         <v>0.10842823445861972</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B34" s="1">
         <v>4502</v>
@@ -1952,18 +1944,18 @@
       <c r="J34" s="1">
         <v>5098</v>
       </c>
-      <c r="K34" s="3">
+      <c r="K34" s="4">
         <f t="shared" si="0"/>
         <v>4855.333333333333</v>
       </c>
-      <c r="L34" s="4">
+      <c r="L34" s="2">
         <f t="shared" si="1"/>
         <v>0.1169085916045508</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B35" s="1">
         <v>4774</v>
@@ -1992,18 +1984,18 @@
       <c r="J35" s="1">
         <v>5511</v>
       </c>
-      <c r="K35" s="3">
+      <c r="K35" s="4">
         <f t="shared" si="0"/>
         <v>5124.5555555555557</v>
       </c>
-      <c r="L35" s="4">
+      <c r="L35" s="2">
         <f t="shared" si="1"/>
         <v>0.13373253493013973</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B36" s="1">
         <v>86862</v>
@@ -2032,18 +2024,18 @@
       <c r="J36" s="1">
         <v>96162</v>
       </c>
-      <c r="K36" s="3">
+      <c r="K36" s="4">
         <f t="shared" si="0"/>
         <v>92205.555555555562</v>
       </c>
-      <c r="L36" s="4">
+      <c r="L36" s="2">
         <f t="shared" si="1"/>
         <v>9.6711798839458407E-2</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B37" s="1">
         <v>58717</v>
@@ -2072,18 +2064,18 @@
       <c r="J37" s="1">
         <v>65002</v>
       </c>
-      <c r="K37" s="3">
+      <c r="K37" s="4">
         <f t="shared" si="0"/>
         <v>62399.111111111109</v>
       </c>
-      <c r="L37" s="4">
+      <c r="L37" s="2">
         <f t="shared" si="1"/>
         <v>9.668933263591889E-2</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B38" s="1">
         <v>14369</v>
@@ -2112,18 +2104,18 @@
       <c r="J38" s="1">
         <v>15803</v>
       </c>
-      <c r="K38" s="3">
+      <c r="K38" s="4">
         <f t="shared" si="0"/>
         <v>15212.222222222223</v>
       </c>
-      <c r="L38" s="4">
+      <c r="L38" s="2">
         <f t="shared" si="1"/>
         <v>9.0742264127064487E-2</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B39" s="1">
         <v>6374</v>
@@ -2152,18 +2144,18 @@
       <c r="J39" s="1">
         <v>6197</v>
       </c>
-      <c r="K39" s="3">
+      <c r="K39" s="4">
         <f t="shared" si="0"/>
         <v>6165.1111111111113</v>
       </c>
-      <c r="L39" s="4">
+      <c r="L39" s="2">
         <f t="shared" si="1"/>
         <v>-2.8562207519767631E-2</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B40" s="1">
         <v>61032</v>
@@ -2192,18 +2184,18 @@
       <c r="J40" s="1">
         <v>65811</v>
       </c>
-      <c r="K40" s="3">
+      <c r="K40" s="4">
         <f t="shared" si="0"/>
         <v>63692.777777777781</v>
       </c>
-      <c r="L40" s="4">
+      <c r="L40" s="2">
         <f t="shared" si="1"/>
         <v>7.2617039704608657E-2</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B41" s="1">
         <v>5958</v>
@@ -2232,18 +2224,18 @@
       <c r="J41" s="1">
         <v>6881</v>
       </c>
-      <c r="K41" s="3">
+      <c r="K41" s="4">
         <f t="shared" si="0"/>
         <v>6467.333333333333</v>
       </c>
-      <c r="L41" s="4">
+      <c r="L41" s="2">
         <f t="shared" si="1"/>
         <v>0.13413748001743933</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B42" s="1">
         <v>14289</v>
@@ -2272,18 +2264,18 @@
       <c r="J42" s="1">
         <v>15841</v>
       </c>
-      <c r="K42" s="3">
+      <c r="K42" s="4">
         <f t="shared" si="0"/>
         <v>15117.111111111111</v>
       </c>
-      <c r="L42" s="4">
+      <c r="L42" s="2">
         <f t="shared" si="1"/>
         <v>9.7973612776971156E-2</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B43" s="1">
         <v>4516</v>
@@ -2312,18 +2304,18 @@
       <c r="J43" s="1">
         <v>4782</v>
       </c>
-      <c r="K43" s="3">
+      <c r="K43" s="4">
         <f t="shared" ref="K43:K52" si="2">(B43+C43+D43+E43+F43+G43+H43+I42+J42)/9</f>
         <v>7072.333333333333</v>
       </c>
-      <c r="L43" s="4">
+      <c r="L43" s="2">
         <f t="shared" si="1"/>
         <v>5.562526139690506E-2</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B44" s="1">
         <v>22355</v>
@@ -2352,18 +2344,18 @@
       <c r="J44" s="1">
         <v>24327</v>
       </c>
-      <c r="K44" s="3">
+      <c r="K44" s="4">
         <f t="shared" si="2"/>
         <v>19224.555555555555</v>
       </c>
-      <c r="L44" s="4">
+      <c r="L44" s="2">
         <f t="shared" si="1"/>
         <v>8.1062194269741442E-2</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B45" s="1">
         <v>75001</v>
@@ -2392,18 +2384,18 @@
       <c r="J45" s="1">
         <v>84056</v>
       </c>
-      <c r="K45" s="3">
+      <c r="K45" s="4">
         <f t="shared" si="2"/>
         <v>66427.888888888891</v>
       </c>
-      <c r="L45" s="4">
+      <c r="L45" s="2">
         <f t="shared" si="1"/>
         <v>0.10772580184638812</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B46" s="1">
         <v>4922</v>
@@ -2432,18 +2424,18 @@
       <c r="J46" s="1">
         <v>5581</v>
       </c>
-      <c r="K46" s="3">
+      <c r="K46" s="4">
         <f t="shared" si="2"/>
         <v>22662.666666666668</v>
       </c>
-      <c r="L46" s="4">
+      <c r="L46" s="2">
         <f t="shared" si="1"/>
         <v>0.11807919727647374</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B47" s="1">
         <v>23540</v>
@@ -2472,18 +2464,18 @@
       <c r="J47" s="1">
         <v>27078</v>
       </c>
-      <c r="K47" s="3">
+      <c r="K47" s="4">
         <f t="shared" si="2"/>
         <v>20842.444444444445</v>
       </c>
-      <c r="L47" s="4">
+      <c r="L47" s="2">
         <f t="shared" si="1"/>
         <v>0.13065957603958933</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B48" s="1">
         <v>2113</v>
@@ -2512,18 +2504,18 @@
       <c r="J48" s="1">
         <v>2307</v>
       </c>
-      <c r="K48" s="3">
+      <c r="K48" s="4">
         <f t="shared" si="2"/>
         <v>7728.1111111111113</v>
       </c>
-      <c r="L48" s="4">
+      <c r="L48" s="2">
         <f t="shared" si="1"/>
         <v>8.4091894234937153E-2</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B49" s="1">
         <v>11733</v>
@@ -2552,18 +2544,18 @@
       <c r="J49" s="1">
         <v>12924</v>
       </c>
-      <c r="K49" s="3">
+      <c r="K49" s="4">
         <f t="shared" si="2"/>
         <v>9989.4444444444453</v>
       </c>
-      <c r="L49" s="4">
+      <c r="L49" s="2">
         <f t="shared" si="1"/>
         <v>9.2154131847725168E-2</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B50" s="1">
         <v>17804</v>
@@ -2592,18 +2584,18 @@
       <c r="J50" s="1">
         <v>17229</v>
       </c>
-      <c r="K50" s="3">
+      <c r="K50" s="4">
         <f t="shared" si="2"/>
         <v>16504.555555555555</v>
       </c>
-      <c r="L50" s="4">
+      <c r="L50" s="2">
         <f t="shared" si="1"/>
         <v>-3.3373962505078646E-2</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B51" s="1">
         <v>8249</v>
@@ -2632,18 +2624,18 @@
       <c r="J51" s="1">
         <v>9226</v>
       </c>
-      <c r="K51" s="3">
+      <c r="K51" s="4">
         <f t="shared" si="2"/>
         <v>10618.111111111111</v>
       </c>
-      <c r="L51" s="4">
+      <c r="L51" s="2">
         <f t="shared" si="1"/>
         <v>0.10589637979622805</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B52" s="1">
         <v>1922</v>
@@ -2672,17 +2664,14 @@
       <c r="J52" s="1">
         <v>1989</v>
       </c>
-      <c r="K52" s="3">
+      <c r="K52" s="4">
         <f t="shared" si="2"/>
         <v>3555.5555555555557</v>
       </c>
-      <c r="L52" s="4">
+      <c r="L52" s="2">
         <f t="shared" si="1"/>
         <v>3.3685268979386625E-2</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="K53" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Data set edit 3
</commit_message>
<xml_diff>
--- a/Facility Staffing Combined.xlsx
+++ b/Facility Staffing Combined.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keros\.venv\Capstone-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31CF0DAA-59BD-4C9E-BDD7-B5ED153FDBCE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C097E90A-0DD6-44DC-83E9-5B578F59AD53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28545" yWindow="15480" windowWidth="16410" windowHeight="11295" xr2:uid="{0B339019-6CC6-4650-AC0A-9ED3E400C083}"/>
   </bookViews>
@@ -224,7 +224,7 @@
     <t>State</t>
   </si>
   <si>
-    <t xml:space="preserve">Employee Average </t>
+    <t>Employee Average</t>
   </si>
 </sst>
 </file>
@@ -260,12 +260,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,7 +582,7 @@
   <dimension ref="A1:L52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+      <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -591,7 +590,7 @@
     <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="3" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -626,7 +625,7 @@
       <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" t="s">
         <v>62</v>
       </c>
       <c r="L1" t="s">
@@ -664,7 +663,7 @@
       <c r="J2">
         <v>625</v>
       </c>
-      <c r="K2" s="4">
+      <c r="K2" s="3">
         <f>(B2+C2+D2+E2+F2+G2+H2+I2+J2)/9</f>
         <v>581.77777777777783</v>
       </c>
@@ -704,7 +703,7 @@
       <c r="J3" s="1">
         <v>20494</v>
       </c>
-      <c r="K3" s="4">
+      <c r="K3" s="3">
         <f t="shared" ref="K3:K42" si="0">(B3+C3+D3+E3+F3+G3+H3+I3+J3)/9</f>
         <v>19238.777777777777</v>
       </c>
@@ -744,7 +743,7 @@
       <c r="J4" s="1">
         <v>15672</v>
       </c>
-      <c r="K4" s="4">
+      <c r="K4" s="3">
         <f t="shared" si="0"/>
         <v>14836.111111111111</v>
       </c>
@@ -784,7 +783,7 @@
       <c r="J5" s="1">
         <v>11421</v>
       </c>
-      <c r="K5" s="4">
+      <c r="K5" s="3">
         <f t="shared" si="0"/>
         <v>10633.444444444445</v>
       </c>
@@ -824,7 +823,7 @@
       <c r="J6" s="1">
         <v>97632</v>
       </c>
-      <c r="K6" s="4">
+      <c r="K6" s="3">
         <f t="shared" si="0"/>
         <v>91049.222222222219</v>
       </c>
@@ -864,7 +863,7 @@
       <c r="J7" s="1">
         <v>14462</v>
       </c>
-      <c r="K7" s="4">
+      <c r="K7" s="3">
         <f t="shared" si="0"/>
         <v>14047.555555555555</v>
       </c>
@@ -904,7 +903,7 @@
       <c r="J8" s="1">
         <v>19836</v>
       </c>
-      <c r="K8" s="4">
+      <c r="K8" s="3">
         <f t="shared" si="0"/>
         <v>18894.222222222223</v>
       </c>
@@ -944,7 +943,7 @@
       <c r="J9" s="1">
         <v>1985</v>
       </c>
-      <c r="K9" s="4">
+      <c r="K9" s="3">
         <f t="shared" si="0"/>
         <v>1976.2222222222222</v>
       </c>
@@ -984,7 +983,7 @@
       <c r="J10" s="1">
         <v>3656</v>
       </c>
-      <c r="K10" s="4">
+      <c r="K10" s="3">
         <f t="shared" si="0"/>
         <v>3475.5555555555557</v>
       </c>
@@ -1024,7 +1023,7 @@
       <c r="J11" s="1">
         <v>71790</v>
       </c>
-      <c r="K11" s="4">
+      <c r="K11" s="3">
         <f t="shared" si="0"/>
         <v>66926.888888888891</v>
       </c>
@@ -1064,7 +1063,7 @@
       <c r="J12" s="1">
         <v>29399</v>
       </c>
-      <c r="K12" s="4">
+      <c r="K12" s="3">
         <f t="shared" si="0"/>
         <v>27631</v>
       </c>
@@ -1104,7 +1103,7 @@
       <c r="J13" s="1">
         <v>3132</v>
       </c>
-      <c r="K13" s="4">
+      <c r="K13" s="3">
         <f t="shared" si="0"/>
         <v>3159.6666666666665</v>
       </c>
@@ -1144,7 +1143,7 @@
       <c r="J14" s="1">
         <v>19803</v>
       </c>
-      <c r="K14" s="4">
+      <c r="K14" s="3">
         <f t="shared" si="0"/>
         <v>19686</v>
       </c>
@@ -1184,7 +1183,7 @@
       <c r="J15" s="1">
         <v>3944</v>
       </c>
-      <c r="K15" s="4">
+      <c r="K15" s="3">
         <f t="shared" si="0"/>
         <v>3657.8888888888887</v>
       </c>
@@ -1224,7 +1223,7 @@
       <c r="J16" s="1">
         <v>59909</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="3">
         <f t="shared" si="0"/>
         <v>56573.555555555555</v>
       </c>
@@ -1264,7 +1263,7 @@
       <c r="J17" s="1">
         <v>35111</v>
       </c>
-      <c r="K17" s="4">
+      <c r="K17" s="3">
         <f t="shared" si="0"/>
         <v>33906.777777777781</v>
       </c>
@@ -1304,7 +1303,7 @@
       <c r="J18" s="1">
         <v>14676</v>
       </c>
-      <c r="K18" s="4">
+      <c r="K18" s="3">
         <f t="shared" si="0"/>
         <v>14469.888888888889</v>
       </c>
@@ -1344,7 +1343,7 @@
       <c r="J19" s="1">
         <v>20422</v>
       </c>
-      <c r="K19" s="4">
+      <c r="K19" s="3">
         <f t="shared" si="0"/>
         <v>20069.666666666668</v>
       </c>
@@ -1384,7 +1383,7 @@
       <c r="J20" s="1">
         <v>22555</v>
       </c>
-      <c r="K20" s="4">
+      <c r="K20" s="3">
         <f t="shared" si="0"/>
         <v>21796.555555555555</v>
       </c>
@@ -1424,7 +1423,7 @@
       <c r="J21" s="1">
         <v>32586</v>
       </c>
-      <c r="K21" s="4">
+      <c r="K21" s="3">
         <f t="shared" si="0"/>
         <v>31527.888888888891</v>
       </c>
@@ -1464,7 +1463,7 @@
       <c r="J22" s="1">
         <v>22486</v>
       </c>
-      <c r="K22" s="4">
+      <c r="K22" s="3">
         <f t="shared" si="0"/>
         <v>21272.888888888891</v>
       </c>
@@ -1504,7 +1503,7 @@
       <c r="J23" s="1">
         <v>5092</v>
       </c>
-      <c r="K23" s="4">
+      <c r="K23" s="3">
         <f t="shared" si="0"/>
         <v>4887.1111111111113</v>
       </c>
@@ -1544,7 +1543,7 @@
       <c r="J24" s="1">
         <v>33370</v>
       </c>
-      <c r="K24" s="4">
+      <c r="K24" s="3">
         <f t="shared" si="0"/>
         <v>31645.777777777777</v>
       </c>
@@ -1584,7 +1583,7 @@
       <c r="J25" s="1">
         <v>19942</v>
       </c>
-      <c r="K25" s="4">
+      <c r="K25" s="3">
         <f t="shared" si="0"/>
         <v>19658.444444444445</v>
       </c>
@@ -1624,7 +1623,7 @@
       <c r="J26" s="1">
         <v>33468</v>
       </c>
-      <c r="K26" s="4">
+      <c r="K26" s="3">
         <f t="shared" si="0"/>
         <v>31743.222222222223</v>
       </c>
@@ -1664,7 +1663,7 @@
       <c r="J27" s="1">
         <v>14139</v>
       </c>
-      <c r="K27" s="4">
+      <c r="K27" s="3">
         <f t="shared" si="0"/>
         <v>13617</v>
       </c>
@@ -1704,7 +1703,7 @@
       <c r="J28" s="1">
         <v>3172</v>
       </c>
-      <c r="K28" s="4">
+      <c r="K28" s="3">
         <f t="shared" si="0"/>
         <v>3158.6666666666665</v>
       </c>
@@ -1744,7 +1743,7 @@
       <c r="J29" s="1">
         <v>32832</v>
       </c>
-      <c r="K29" s="4">
+      <c r="K29" s="3">
         <f t="shared" si="0"/>
         <v>31356</v>
       </c>
@@ -1784,7 +1783,7 @@
       <c r="J30" s="1">
         <v>4457</v>
       </c>
-      <c r="K30" s="4">
+      <c r="K30" s="3">
         <f t="shared" si="0"/>
         <v>4445.666666666667</v>
       </c>
@@ -1824,7 +1823,7 @@
       <c r="J31" s="1">
         <v>9405</v>
       </c>
-      <c r="K31" s="4">
+      <c r="K31" s="3">
         <f t="shared" si="0"/>
         <v>9359.2222222222226</v>
       </c>
@@ -1864,7 +1863,7 @@
       <c r="J32" s="1">
         <v>5662</v>
       </c>
-      <c r="K32" s="4">
+      <c r="K32" s="3">
         <f t="shared" si="0"/>
         <v>5484.7777777777774</v>
       </c>
@@ -1904,7 +1903,7 @@
       <c r="J33" s="1">
         <v>39427</v>
       </c>
-      <c r="K33" s="4">
+      <c r="K33" s="3">
         <f t="shared" si="0"/>
         <v>37192.111111111109</v>
       </c>
@@ -1944,7 +1943,7 @@
       <c r="J34" s="1">
         <v>5098</v>
       </c>
-      <c r="K34" s="4">
+      <c r="K34" s="3">
         <f t="shared" si="0"/>
         <v>4855.333333333333</v>
       </c>
@@ -1984,7 +1983,7 @@
       <c r="J35" s="1">
         <v>5511</v>
       </c>
-      <c r="K35" s="4">
+      <c r="K35" s="3">
         <f t="shared" si="0"/>
         <v>5124.5555555555557</v>
       </c>
@@ -2024,7 +2023,7 @@
       <c r="J36" s="1">
         <v>96162</v>
       </c>
-      <c r="K36" s="4">
+      <c r="K36" s="3">
         <f t="shared" si="0"/>
         <v>92205.555555555562</v>
       </c>
@@ -2064,7 +2063,7 @@
       <c r="J37" s="1">
         <v>65002</v>
       </c>
-      <c r="K37" s="4">
+      <c r="K37" s="3">
         <f t="shared" si="0"/>
         <v>62399.111111111109</v>
       </c>
@@ -2104,7 +2103,7 @@
       <c r="J38" s="1">
         <v>15803</v>
       </c>
-      <c r="K38" s="4">
+      <c r="K38" s="3">
         <f t="shared" si="0"/>
         <v>15212.222222222223</v>
       </c>
@@ -2144,7 +2143,7 @@
       <c r="J39" s="1">
         <v>6197</v>
       </c>
-      <c r="K39" s="4">
+      <c r="K39" s="3">
         <f t="shared" si="0"/>
         <v>6165.1111111111113</v>
       </c>
@@ -2184,7 +2183,7 @@
       <c r="J40" s="1">
         <v>65811</v>
       </c>
-      <c r="K40" s="4">
+      <c r="K40" s="3">
         <f t="shared" si="0"/>
         <v>63692.777777777781</v>
       </c>
@@ -2224,7 +2223,7 @@
       <c r="J41" s="1">
         <v>6881</v>
       </c>
-      <c r="K41" s="4">
+      <c r="K41" s="3">
         <f t="shared" si="0"/>
         <v>6467.333333333333</v>
       </c>
@@ -2264,7 +2263,7 @@
       <c r="J42" s="1">
         <v>15841</v>
       </c>
-      <c r="K42" s="4">
+      <c r="K42" s="3">
         <f t="shared" si="0"/>
         <v>15117.111111111111</v>
       </c>
@@ -2304,7 +2303,7 @@
       <c r="J43" s="1">
         <v>4782</v>
       </c>
-      <c r="K43" s="4">
+      <c r="K43" s="3">
         <f t="shared" ref="K43:K52" si="2">(B43+C43+D43+E43+F43+G43+H43+I42+J42)/9</f>
         <v>7072.333333333333</v>
       </c>
@@ -2344,7 +2343,7 @@
       <c r="J44" s="1">
         <v>24327</v>
       </c>
-      <c r="K44" s="4">
+      <c r="K44" s="3">
         <f t="shared" si="2"/>
         <v>19224.555555555555</v>
       </c>
@@ -2384,7 +2383,7 @@
       <c r="J45" s="1">
         <v>84056</v>
       </c>
-      <c r="K45" s="4">
+      <c r="K45" s="3">
         <f t="shared" si="2"/>
         <v>66427.888888888891</v>
       </c>
@@ -2424,7 +2423,7 @@
       <c r="J46" s="1">
         <v>5581</v>
       </c>
-      <c r="K46" s="4">
+      <c r="K46" s="3">
         <f t="shared" si="2"/>
         <v>22662.666666666668</v>
       </c>
@@ -2464,7 +2463,7 @@
       <c r="J47" s="1">
         <v>27078</v>
       </c>
-      <c r="K47" s="4">
+      <c r="K47" s="3">
         <f t="shared" si="2"/>
         <v>20842.444444444445</v>
       </c>
@@ -2504,7 +2503,7 @@
       <c r="J48" s="1">
         <v>2307</v>
       </c>
-      <c r="K48" s="4">
+      <c r="K48" s="3">
         <f t="shared" si="2"/>
         <v>7728.1111111111113</v>
       </c>
@@ -2544,7 +2543,7 @@
       <c r="J49" s="1">
         <v>12924</v>
       </c>
-      <c r="K49" s="4">
+      <c r="K49" s="3">
         <f t="shared" si="2"/>
         <v>9989.4444444444453</v>
       </c>
@@ -2584,7 +2583,7 @@
       <c r="J50" s="1">
         <v>17229</v>
       </c>
-      <c r="K50" s="4">
+      <c r="K50" s="3">
         <f t="shared" si="2"/>
         <v>16504.555555555555</v>
       </c>
@@ -2624,7 +2623,7 @@
       <c r="J51" s="1">
         <v>9226</v>
       </c>
-      <c r="K51" s="4">
+      <c r="K51" s="3">
         <f t="shared" si="2"/>
         <v>10618.111111111111</v>
       </c>
@@ -2664,7 +2663,7 @@
       <c r="J52" s="1">
         <v>1989</v>
       </c>
-      <c r="K52" s="4">
+      <c r="K52" s="3">
         <f t="shared" si="2"/>
         <v>3555.5555555555557</v>
       </c>

</xml_diff>